<commit_message>
Add target raw data
</commit_message>
<xml_diff>
--- a/data/raw/base_casamentos.xlsx
+++ b/data/raw/base_casamentos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodto\OneDrive\04 Profissional\03 Letivas\04 FGV\02 MBA BA BigData\04 Disciplinas\08 Matrizes e Clusters\05 Trabalho em Grupo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\FGV\04_Modulos\07 - Metodos Matriciais e Analise de Clusters\Matrix-Methods-Cluster-Analysis\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{B49F08CB-9581-46DE-A758-4458CBA7C297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{57B699AA-2846-4685-B523-3BEC755A3313}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{B49F08CB-9581-46DE-A758-4458CBA7C297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9AE1DF23-9D1C-4514-BA4D-0C39EFD6FF03}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{676442C3-E9B8-483E-A436-3C4D2A4AA6FA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{676442C3-E9B8-483E-A436-3C4D2A4AA6FA}"/>
   </bookViews>
   <sheets>
     <sheet name="CASAMENTOS" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C2C69E-7283-4C7B-AFAE-BDCC89462597}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>